<commit_message>
added my list of soft and hardware
</commit_message>
<xml_diff>
--- a/documenten/kerntaak_1/1.5/materialenlijst/materialenlijst_0.1.xlsx
+++ b/documenten/kerntaak_1/1.5/materialenlijst/materialenlijst_0.1.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\PvB\exam\documenten\kerntaak_1\1.5\materialenlijst\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\did-you-had-a-good-day\documenten\kerntaak_1\1.5\materialenlijst\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36CC3ADC-3C3C-4399-B9FE-E6A113217DD0}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12216" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
   <si>
     <t>Beschrijving</t>
   </si>
@@ -80,13 +81,58 @@
     <t>Google Chrome</t>
   </si>
   <si>
-    <t>Discord</t>
+    <t>10.0.16299 Build 16299</t>
+  </si>
+  <si>
+    <t>Intel(R) Core(TM) i5-4200U CPU @ 1.60GHz, 2301 MHz, 2 core('s), 4 logische processor(s)</t>
+  </si>
+  <si>
+    <t>Graphics Chipset</t>
+  </si>
+  <si>
+    <t>AMD Radeon R7 M265 Series</t>
+  </si>
+  <si>
+    <t>sublime</t>
+  </si>
+  <si>
+    <t>nodeJS</t>
+  </si>
+  <si>
+    <t>VeuJS</t>
+  </si>
+  <si>
+    <t>git</t>
+  </si>
+  <si>
+    <t>gitkraken</t>
+  </si>
+  <si>
+    <t>3.0.6</t>
+  </si>
+  <si>
+    <t>65.0.3325.181</t>
+  </si>
+  <si>
+    <t>2.10.0.windows.1</t>
+  </si>
+  <si>
+    <t>3.5.1</t>
+  </si>
+  <si>
+    <t>v8.6.0</t>
+  </si>
+  <si>
+    <t>2.5.16</t>
+  </si>
+  <si>
+    <t>build 3126</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -457,25 +503,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:D31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B3:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="87.140625" customWidth="1"/>
-    <col min="3" max="3" width="55.7109375" customWidth="1"/>
-    <col min="4" max="4" width="54.7109375" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
-    <col min="6" max="6" width="40.85546875" customWidth="1"/>
-    <col min="7" max="7" width="61.42578125" customWidth="1"/>
-    <col min="8" max="8" width="35.7109375" customWidth="1"/>
+    <col min="2" max="2" width="87.109375" customWidth="1"/>
+    <col min="3" max="3" width="55.6640625" customWidth="1"/>
+    <col min="4" max="4" width="54.6640625" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" customWidth="1"/>
+    <col min="6" max="6" width="40.88671875" customWidth="1"/>
+    <col min="7" max="7" width="61.44140625" customWidth="1"/>
+    <col min="8" max="8" width="35.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
@@ -486,7 +532,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
@@ -494,7 +540,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -502,7 +548,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>9</v>
       </c>
@@ -513,7 +559,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>12</v>
       </c>
@@ -524,22 +570,22 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>10</v>
       </c>
@@ -547,30 +593,121 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B31" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>13</v>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>